<commit_message>
New test - Product Page.
</commit_message>
<xml_diff>
--- a/IkeaFramework/TestData/Data.xlsx
+++ b/IkeaFramework/TestData/Data.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Product" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,12 +21,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">testuser</t>
   </si>
   <si>
     <t xml:space="preserve">demo123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KIVIK</t>
   </si>
 </sst>
 </file>
@@ -261,7 +265,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -272,6 +276,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -369,7 +377,7 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -395,4 +403,39 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="n">
+        <v>99011429</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new WebElements for checkForLocation().
</commit_message>
<xml_diff>
--- a/IkeaFramework/TestData/Data.xlsx
+++ b/IkeaFramework/TestData/Data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">testuser</t>
   </si>
@@ -29,7 +29,13 @@
     <t xml:space="preserve">demo123</t>
   </si>
   <si>
+    <t xml:space="preserve">PAX</t>
+  </si>
+  <si>
     <t xml:space="preserve">KIVIK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINNMON/ALEX</t>
   </si>
 </sst>
 </file>
@@ -410,7 +416,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -418,15 +424,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="n">
-        <v>99011429</v>
+        <v>19288134</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
+        <v>99011429</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>69222616</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Used @FindBy (how, using) and  List<WebElement> to improve toggleLocation by using toggles.get(16) instead.
</commit_message>
<xml_diff>
--- a/IkeaFramework/TestData/Data.xlsx
+++ b/IkeaFramework/TestData/Data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t xml:space="preserve">testuser</t>
   </si>
@@ -29,13 +29,13 @@
     <t xml:space="preserve">demo123</t>
   </si>
   <si>
-    <t xml:space="preserve">PAX</t>
+    <t xml:space="preserve">LINNMON/ALEX</t>
   </si>
   <si>
     <t xml:space="preserve">KIVIK</t>
   </si>
   <si>
-    <t xml:space="preserve">LINNMON/ALEX</t>
+    <t xml:space="preserve">PAX</t>
   </si>
 </sst>
 </file>
@@ -384,7 +384,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -416,10 +416,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -430,26 +430,34 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="n">
-        <v>19288134</v>
+      <c r="A1" s="0" t="n">
+        <v>69222616</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
         <v>99011429</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>69222616</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
+        <v>19288134</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <v>59931463</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Need to find a better way to check if the WebElement components exists or not.
</commit_message>
<xml_diff>
--- a/IkeaFramework/TestData/Data.xlsx
+++ b/IkeaFramework/TestData/Data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t xml:space="preserve">testuser</t>
   </si>
@@ -29,10 +29,13 @@
     <t xml:space="preserve">demo123</t>
   </si>
   <si>
+    <t xml:space="preserve">ALEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KIVIK</t>
+  </si>
+  <si>
     <t xml:space="preserve">LINNMON/ALEX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KIVIK</t>
   </si>
   <si>
     <t xml:space="preserve">PAX</t>
@@ -384,7 +387,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="A1:B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -419,7 +422,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -430,8 +433,8 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>69222616</v>
+      <c r="A1" s="3" t="n">
+        <v>40260717</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
@@ -445,12 +448,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>69222616</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
         <v>19288134</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -458,7 +469,7 @@
         <v>59931463</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Product Page test. Needs to add assertions for productDetails().
</commit_message>
<xml_diff>
--- a/IkeaFramework/TestData/Data.xlsx
+++ b/IkeaFramework/TestData/Data.xlsx
@@ -29,6 +29,9 @@
     <t xml:space="preserve">demo123</t>
   </si>
   <si>
+    <t xml:space="preserve">PAX</t>
+  </si>
+  <si>
     <t xml:space="preserve">ALEX</t>
   </si>
   <si>
@@ -36,9 +39,6 @@
   </si>
   <si>
     <t xml:space="preserve">LINNMON/ALEX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAX</t>
   </si>
 </sst>
 </file>
@@ -387,7 +387,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -419,10 +419,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -434,10 +434,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="n">
-        <v>40260717</v>
+        <v>59931463</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
+        <v>40260717</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -445,7 +453,7 @@
         <v>99011429</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -453,7 +461,7 @@
         <v>69222616</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -461,15 +469,7 @@
         <v>19288134</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
-        <v>59931463</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved wishlistApp() and added rowCounter(String sheetName).
</commit_message>
<xml_diff>
--- a/IkeaFramework/TestData/Data.xlsx
+++ b/IkeaFramework/TestData/Data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t xml:space="preserve">testuser</t>
   </si>
@@ -36,10 +36,13 @@
     <t xml:space="preserve">KIVIK</t>
   </si>
   <si>
+    <t xml:space="preserve">PAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LÅNGFJÄLL</t>
+  </si>
+  <si>
     <t xml:space="preserve">LINNMON/ALEX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAX</t>
   </si>
   <si>
     <t xml:space="preserve">נתניה</t>
@@ -432,10 +435,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -463,26 +466,34 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>19288134</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>59931463</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>39252515</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
         <v>69222616</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
-        <v>19288134</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
-        <v>59931463</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
+      <c r="B6" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -514,22 +525,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved Helper with robotScrollUp().
</commit_message>
<xml_diff>
--- a/IkeaFramework/TestData/Data.xlsx
+++ b/IkeaFramework/TestData/Data.xlsx
@@ -403,7 +403,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A4:B6 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -438,7 +438,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -515,7 +515,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>